<commit_message>
fix TypeError, refine logic, add try catch, add "江西"
</commit_message>
<xml_diff>
--- a/漫展信息/丽水-漫展信息.xlsx
+++ b/漫展信息/丽水-漫展信息.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,15 +472,10 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>是否有舞台（字符串匹配）</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>Cover</t>
         </is>
@@ -511,20 +506,17 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="G2" t="n">
         <v>45</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202311/lP5IkqWn1699431829470.jpeg</t>
         </is>
@@ -555,20 +547,17 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="G3" t="n">
         <v>50</v>
       </c>
-      <c r="H3" t="b">
-        <v>0</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/rTvQio211704877379770.jpeg</t>
         </is>
@@ -599,20 +588,17 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G4" t="n">
         <v>45</v>
       </c>
-      <c r="H4" t="b">
-        <v>0</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
         <is>
           <t>//i0.hdslb.com/bfs/openplatform/202401/LbqTNkvq1705561884633.png</t>
         </is>
@@ -643,20 +629,17 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="G5" t="n">
         <v>45</v>
       </c>
-      <c r="H5" t="b">
-        <v>0</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202312/ee5hLUN61702276208812.jpeg</t>
         </is>
@@ -673,7 +656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -717,15 +700,10 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>是否有舞台（字符串匹配）</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>Cover</t>
         </is>
@@ -742,7 +720,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,15 +764,10 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>是否有舞台（字符串匹配）</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>Cover</t>
         </is>
@@ -811,7 +784,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,15 +828,10 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>是否有舞台（字符串匹配）</t>
+          <t>Link</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
         <is>
           <t>Cover</t>
         </is>
@@ -894,20 +862,17 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="G2" t="n">
         <v>45</v>
       </c>
-      <c r="H2" t="b">
-        <v>0</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=78294</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202311/lP5IkqWn1699431829470.jpeg</t>
         </is>
@@ -938,20 +903,17 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="G3" t="n">
         <v>50</v>
       </c>
-      <c r="H3" t="b">
-        <v>0</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=80714</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
         <is>
           <t>//i2.hdslb.com/bfs/openplatform/202401/rTvQio211704877379770.jpeg</t>
         </is>
@@ -982,20 +944,17 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="G4" t="n">
         <v>45</v>
       </c>
-      <c r="H4" t="b">
-        <v>0</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=81032</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
         <is>
           <t>//i0.hdslb.com/bfs/openplatform/202401/LbqTNkvq1705561884633.png</t>
         </is>
@@ -1026,20 +985,17 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="G5" t="n">
         <v>45</v>
       </c>
-      <c r="H5" t="b">
-        <v>0</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>https://show.bilibili.com/platform/detail.html?id=79437</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
         <is>
           <t>//i1.hdslb.com/bfs/openplatform/202312/ee5hLUN61702276208812.jpeg</t>
         </is>

</xml_diff>